<commit_message>
09-21-2021 : Logger completed preparing 2nd test case facing issue on running testNG file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -1,40 +1,403 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView windowWidth="24225" windowHeight="12495"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>postCode</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -42,18 +405,312 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -336,42 +993,81 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="17.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="12.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="22.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>123456</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
09-24-2021 : Excel sheet working now , ReportNG integration is in Progress
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12495"/>
+    <workbookView windowWidth="15915" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>firstName</t>
   </si>
@@ -27,10 +27,28 @@
     <t>postCode</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>Rahul</t>
   </si>
   <si>
     <t>Singh</t>
+  </si>
+  <si>
+    <t>Customer added successfully with customer id :6</t>
+  </si>
+  <si>
+    <t>raj</t>
+  </si>
+  <si>
+    <t>Customer added successfully with customer id :7</t>
+  </si>
+  <si>
+    <t>raju</t>
+  </si>
+  <si>
+    <t>Customer added successfully with customer id :8</t>
   </si>
 </sst>
 </file>
@@ -38,12 +56,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +70,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -59,6 +85,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -67,62 +108,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,6 +124,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -144,45 +139,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,7 +156,59 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,13 +223,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +325,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,157 +403,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,21 +414,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -432,17 +428,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -471,6 +456,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -488,9 +497,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,148 +517,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -999,20 +1010,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="17.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="12.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="22.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="44.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1022,16 +1034,50 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>123456</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>56667</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>66755</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>